<commit_message>
added necro hood fixed a time-bug with equipment
</commit_message>
<xml_diff>
--- a/res/convenience/items.xlsx
+++ b/res/convenience/items.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="126">
   <si>
     <t>Item ID</t>
   </si>
@@ -380,6 +380,18 @@
   </si>
   <si>
     <t>2, 1</t>
+  </si>
+  <si>
+    <t>itd_head_necrot3</t>
+  </si>
+  <si>
+    <t>it_eq_head_necrot3</t>
+  </si>
+  <si>
+    <t>0, 200</t>
+  </si>
+  <si>
+    <t>res/assets/equipment/head/spritesheet_head_necrot3.png</t>
   </si>
 </sst>
 </file>
@@ -1202,10 +1214,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AG17"/>
+  <dimension ref="A1:AG18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="Y19" sqref="Y19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1845,7 +1857,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="17" spans="1:24">
+    <row r="17" spans="1:25">
       <c r="A17" t="s">
         <v>79</v>
       </c>
@@ -1869,6 +1881,41 @@
       </c>
       <c r="X17">
         <v>1000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:25">
+      <c r="A18" t="s">
+        <v>123</v>
+      </c>
+      <c r="B18" t="s">
+        <v>122</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18" t="s">
+        <v>124</v>
+      </c>
+      <c r="E18">
+        <v>120</v>
+      </c>
+      <c r="F18">
+        <v>10</v>
+      </c>
+      <c r="M18">
+        <v>10</v>
+      </c>
+      <c r="O18">
+        <v>5</v>
+      </c>
+      <c r="R18">
+        <v>10</v>
+      </c>
+      <c r="S18">
+        <v>10</v>
+      </c>
+      <c r="Y18" t="s">
+        <v>125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added item: necrot3 back stat: critical gets now translated correctly
</commit_message>
<xml_diff>
--- a/res/convenience/items.xlsx
+++ b/res/convenience/items.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="130">
   <si>
     <t>Item ID</t>
   </si>
@@ -392,6 +392,18 @@
   </si>
   <si>
     <t>res/assets/equipment/head/spritesheet_head_necrot3.png</t>
+  </si>
+  <si>
+    <t>it_eq_back_necrot3</t>
+  </si>
+  <si>
+    <t>itd_back_necrot3</t>
+  </si>
+  <si>
+    <t>50, 200</t>
+  </si>
+  <si>
+    <t>res/assets/equipment/back/spritesheet_back_necrot3.png</t>
   </si>
 </sst>
 </file>
@@ -1214,10 +1226,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AG18"/>
+  <dimension ref="A1:AG19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Y19" sqref="Y19"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="AA23" sqref="AA23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1918,6 +1930,47 @@
         <v>125</v>
       </c>
     </row>
+    <row r="19" spans="1:25">
+      <c r="A19" t="s">
+        <v>126</v>
+      </c>
+      <c r="B19" t="s">
+        <v>127</v>
+      </c>
+      <c r="C19">
+        <v>7</v>
+      </c>
+      <c r="D19" t="s">
+        <v>128</v>
+      </c>
+      <c r="E19">
+        <v>150</v>
+      </c>
+      <c r="F19">
+        <v>20</v>
+      </c>
+      <c r="H19">
+        <v>20</v>
+      </c>
+      <c r="I19">
+        <v>10</v>
+      </c>
+      <c r="M19">
+        <v>10</v>
+      </c>
+      <c r="O19">
+        <v>10</v>
+      </c>
+      <c r="R19">
+        <v>10</v>
+      </c>
+      <c r="S19">
+        <v>10</v>
+      </c>
+      <c r="Y19" t="s">
+        <v>129</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
added equipment necrot3 body
</commit_message>
<xml_diff>
--- a/res/convenience/items.xlsx
+++ b/res/convenience/items.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="134">
   <si>
     <t>Item ID</t>
   </si>
@@ -404,6 +404,18 @@
   </si>
   <si>
     <t>res/assets/equipment/back/spritesheet_back_necrot3.png</t>
+  </si>
+  <si>
+    <t>itd_body_necrot3</t>
+  </si>
+  <si>
+    <t>it_eq_body_necrot3</t>
+  </si>
+  <si>
+    <t>100, 200</t>
+  </si>
+  <si>
+    <t>res/assets/equipment/body/spritesheet_body_necrot3.png</t>
   </si>
 </sst>
 </file>
@@ -1226,10 +1238,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AG19"/>
+  <dimension ref="A1:AG20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="AA23" sqref="AA23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AB21" sqref="AB21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1971,6 +1983,59 @@
         <v>129</v>
       </c>
     </row>
+    <row r="20" spans="1:25">
+      <c r="A20" t="s">
+        <v>131</v>
+      </c>
+      <c r="B20" t="s">
+        <v>130</v>
+      </c>
+      <c r="C20">
+        <v>5</v>
+      </c>
+      <c r="D20" t="s">
+        <v>132</v>
+      </c>
+      <c r="E20">
+        <v>200</v>
+      </c>
+      <c r="F20">
+        <v>30</v>
+      </c>
+      <c r="G20">
+        <v>1</v>
+      </c>
+      <c r="H20">
+        <v>30</v>
+      </c>
+      <c r="K20">
+        <v>10</v>
+      </c>
+      <c r="L20">
+        <v>10</v>
+      </c>
+      <c r="M20">
+        <v>20</v>
+      </c>
+      <c r="O20">
+        <v>30</v>
+      </c>
+      <c r="P20">
+        <v>5</v>
+      </c>
+      <c r="Q20">
+        <v>5</v>
+      </c>
+      <c r="R20">
+        <v>5</v>
+      </c>
+      <c r="S20">
+        <v>5</v>
+      </c>
+      <c r="Y20" t="s">
+        <v>133</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
tweaked weapon & interface logic added new equipment items
</commit_message>
<xml_diff>
--- a/res/convenience/items.xlsx
+++ b/res/convenience/items.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="142">
   <si>
     <t>Item ID</t>
   </si>
@@ -416,6 +416,30 @@
   </si>
   <si>
     <t>res/assets/equipment/body/spritesheet_body_necrot3.png</t>
+  </si>
+  <si>
+    <t>res/assets/equipment/head/spritesheet_head_rafishat.png</t>
+  </si>
+  <si>
+    <t>0, 250</t>
+  </si>
+  <si>
+    <t>it_eq_rafishat</t>
+  </si>
+  <si>
+    <t>itd_rafishat</t>
+  </si>
+  <si>
+    <t>res/assets/equipment/head/spritesheet_head_divinet3.png</t>
+  </si>
+  <si>
+    <t>it_eq_head_divinet3</t>
+  </si>
+  <si>
+    <t>itd_head_divinet3</t>
+  </si>
+  <si>
+    <t>150, 200</t>
   </si>
 </sst>
 </file>
@@ -1238,10 +1262,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AG20"/>
+  <dimension ref="A1:AG22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AB21" sqref="AB21"/>
+      <selection activeCell="S22" sqref="S22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2036,6 +2060,85 @@
         <v>133</v>
       </c>
     </row>
+    <row r="21" spans="1:25">
+      <c r="A21" t="s">
+        <v>136</v>
+      </c>
+      <c r="B21" t="s">
+        <v>137</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21" t="s">
+        <v>135</v>
+      </c>
+      <c r="E21">
+        <v>10</v>
+      </c>
+      <c r="H21">
+        <v>-20</v>
+      </c>
+      <c r="I21">
+        <v>5</v>
+      </c>
+      <c r="O21">
+        <v>2</v>
+      </c>
+      <c r="P21">
+        <v>2</v>
+      </c>
+      <c r="Q21">
+        <v>1</v>
+      </c>
+      <c r="Y21" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="22" spans="1:25">
+      <c r="A22" t="s">
+        <v>139</v>
+      </c>
+      <c r="B22" t="s">
+        <v>140</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22" t="s">
+        <v>141</v>
+      </c>
+      <c r="E22">
+        <v>120</v>
+      </c>
+      <c r="F22">
+        <v>10</v>
+      </c>
+      <c r="G22">
+        <v>1</v>
+      </c>
+      <c r="H22">
+        <v>20</v>
+      </c>
+      <c r="I22">
+        <v>10</v>
+      </c>
+      <c r="K22">
+        <v>10</v>
+      </c>
+      <c r="N22">
+        <v>10</v>
+      </c>
+      <c r="O22">
+        <v>2</v>
+      </c>
+      <c r="S22">
+        <v>10</v>
+      </c>
+      <c r="Y22" t="s">
+        <v>138</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
added item: lesser healing potion attacking an enemy will break cendrics invisibility npc dialogue heads in trade mode are now scaled to fit using the quickslot via mouse click will now lock correctly resolved a pointer mess in merchant windows
</commit_message>
<xml_diff>
--- a/res/convenience/items.xlsx
+++ b/res/convenience/items.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="148">
   <si>
     <t>Item ID</t>
   </si>
@@ -440,6 +440,24 @@
   </si>
   <si>
     <t>150, 200</t>
+  </si>
+  <si>
+    <t>it_fo_lesserhealingpotion</t>
+  </si>
+  <si>
+    <t>itd_lesserhealingpotion</t>
+  </si>
+  <si>
+    <t>100, 100</t>
+  </si>
+  <si>
+    <t>-15, -2</t>
+  </si>
+  <si>
+    <t>20, 46</t>
+  </si>
+  <si>
+    <t>100, 100, 50, 50</t>
   </si>
 </sst>
 </file>
@@ -1262,10 +1280,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AG22"/>
+  <dimension ref="A1:AG23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S22" sqref="S22"/>
+      <selection activeCell="X25" sqref="X25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1835,7 +1853,7 @@
         <v>71</v>
       </c>
       <c r="E14">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="U14" s="1" t="s">
         <v>86</v>
@@ -2137,6 +2155,41 @@
       </c>
       <c r="Y22" t="s">
         <v>138</v>
+      </c>
+    </row>
+    <row r="23" spans="1:25">
+      <c r="A23" t="s">
+        <v>142</v>
+      </c>
+      <c r="B23" t="s">
+        <v>143</v>
+      </c>
+      <c r="C23">
+        <v>8</v>
+      </c>
+      <c r="D23" t="s">
+        <v>144</v>
+      </c>
+      <c r="E23">
+        <v>15</v>
+      </c>
+      <c r="G23">
+        <v>5</v>
+      </c>
+      <c r="T23">
+        <v>5</v>
+      </c>
+      <c r="U23" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="V23" t="s">
+        <v>146</v>
+      </c>
+      <c r="W23" t="s">
+        <v>147</v>
+      </c>
+      <c r="X23">
+        <v>1000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
refactoring and added support for animated tiles from tiled
</commit_message>
<xml_diff>
--- a/res/convenience/items.xlsx
+++ b/res/convenience/items.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="151">
   <si>
     <t>Item ID</t>
   </si>
@@ -458,6 +458,15 @@
   </si>
   <si>
     <t>100, 100, 50, 50</t>
+  </si>
+  <si>
+    <t>itd_rawmeat</t>
+  </si>
+  <si>
+    <t>200, 50</t>
+  </si>
+  <si>
+    <t>it_fo_rawmeat</t>
   </si>
 </sst>
 </file>
@@ -1280,10 +1289,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AG23"/>
+  <dimension ref="A1:AG24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="X25" sqref="X25"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2192,6 +2201,32 @@
         <v>1000</v>
       </c>
     </row>
+    <row r="24" spans="1:25">
+      <c r="A24" t="s">
+        <v>150</v>
+      </c>
+      <c r="B24" t="s">
+        <v>148</v>
+      </c>
+      <c r="C24">
+        <v>8</v>
+      </c>
+      <c r="D24" t="s">
+        <v>149</v>
+      </c>
+      <c r="E24">
+        <v>2</v>
+      </c>
+      <c r="G24">
+        <v>2</v>
+      </c>
+      <c r="J24">
+        <v>5</v>
+      </c>
+      <c r="T24">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>